<commit_message>
add new excel and func
</commit_message>
<xml_diff>
--- a/server.xlsx
+++ b/server.xlsx
@@ -1522,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O171"/>
+  <dimension ref="A1:O189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2177,183 +2177,237 @@
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -2616,6 +2670,114 @@
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="3"/>
+      <c r="B172" s="3"/>
+      <c r="C172" s="3"/>
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="3"/>
+      <c r="B173" s="3"/>
+      <c r="C173" s="3"/>
+      <c r="D173" s="3"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="3"/>
+      <c r="B174" s="3"/>
+      <c r="C174" s="3"/>
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="3"/>
+      <c r="B175" s="3"/>
+      <c r="C175" s="3"/>
+      <c r="D175" s="3"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="3"/>
+      <c r="B176" s="3"/>
+      <c r="C176" s="3"/>
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="3"/>
+      <c r="B177" s="3"/>
+      <c r="C177" s="3"/>
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="3"/>
+      <c r="B178" s="3"/>
+      <c r="C178" s="3"/>
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="3"/>
+      <c r="B179" s="3"/>
+      <c r="C179" s="3"/>
+      <c r="D179" s="3"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="3"/>
+      <c r="B180" s="3"/>
+      <c r="C180" s="3"/>
+      <c r="D180" s="3"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="3"/>
+      <c r="B181" s="3"/>
+      <c r="C181" s="3"/>
+      <c r="D181" s="3"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="3"/>
+      <c r="B182" s="3"/>
+      <c r="C182" s="3"/>
+      <c r="D182" s="3"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="3"/>
+      <c r="B183" s="3"/>
+      <c r="C183" s="3"/>
+      <c r="D183" s="3"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="3"/>
+      <c r="B184" s="3"/>
+      <c r="C184" s="3"/>
+      <c r="D184" s="3"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="3"/>
+      <c r="B185" s="3"/>
+      <c r="C185" s="3"/>
+      <c r="D185" s="3"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="3"/>
+      <c r="B186" s="3"/>
+      <c r="C186" s="3"/>
+      <c r="D186" s="3"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="3"/>
+      <c r="B187" s="3"/>
+      <c r="C187" s="3"/>
+      <c r="D187" s="3"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="3"/>
+      <c r="B188" s="3"/>
+      <c r="C188" s="3"/>
+      <c r="D188" s="3"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="3"/>
+      <c r="B189" s="3"/>
+      <c r="C189" s="3"/>
+      <c r="D189" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>